<commit_message>
Select format bug resolved
</commit_message>
<xml_diff>
--- a/Cinema/movies.xlsx
+++ b/Cinema/movies.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hirne\Documents\GitHub\RpaCinemaProject\Cinema\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan\Documents\GitHub\RpaCinemaProject\Cinema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFA6078-C1CD-480D-819E-70114A451785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30705" yWindow="135" windowWidth="21600" windowHeight="11385" xr2:uid="{F818FDDF-5810-4FFB-939E-69EEA39713A8}"/>
+    <workbookView xWindow="30705" yWindow="135" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>CLIFFORD, MARELE CAINE ROSU</t>
   </si>
@@ -58,9 +57,6 @@
     <t>VANATORII DE FANTOME: MOSTENIREA</t>
   </si>
   <si>
-    <t>Rating: 4.9/10</t>
-  </si>
-  <si>
     <t>Rating: 6/10</t>
   </si>
   <si>
@@ -88,13 +84,28 @@
     <t>Rating: 2.5/10</t>
   </si>
   <si>
-    <t>Rating: 6.5/10</t>
+    <t>CASA GUCCI</t>
+  </si>
+  <si>
+    <t>Rating: 6.9/10</t>
+  </si>
+  <si>
+    <t>Rating: 6.4/10</t>
+  </si>
+  <si>
+    <t>Rating: 7.4/10</t>
+  </si>
+  <si>
+    <t>355</t>
+  </si>
+  <si>
+    <t>Rating: 4.8/10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,8 +135,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,117 +451,193 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B917C1-B205-4FF8-9E09-2669AB534894}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>355</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>6</v>
-      </c>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>